<commit_message>
P10 Trial Run Calculate total cost of order
</commit_message>
<xml_diff>
--- a/P10/Scrum_Sprint_4.xlsx
+++ b/P10/Scrum_Sprint_4.xlsx
@@ -753,7 +753,7 @@
     <t xml:space="preserve">Write – Design Graph</t>
   </si>
   <si>
-    <t xml:space="preserve">git commit -m "P07 Trial Run Calculate total cost of order</t>
+    <t xml:space="preserve">git commit -m "P10 Trial Run Calculate total cost of order”</t>
   </si>
   <si>
     <t xml:space="preserve">BONUS</t>
@@ -1266,7 +1266,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1418,11 +1418,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="28358404"/>
-        <c:axId val="10899167"/>
+        <c:axId val="80301376"/>
+        <c:axId val="78889942"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="28358404"/>
+        <c:axId val="80301376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1489,12 +1489,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10899167"/>
+        <c:crossAx val="78889942"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="10899167"/>
+        <c:axId val="78889942"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1569,7 +1569,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28358404"/>
+        <c:crossAx val="80301376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1596,7 +1596,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1724,11 +1724,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="75141790"/>
-        <c:axId val="60977321"/>
+        <c:axId val="82286716"/>
+        <c:axId val="55825780"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="75141790"/>
+        <c:axId val="82286716"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1793,7 +1793,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60977321"/>
+        <c:crossAx val="55825780"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1801,7 +1801,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60977321"/>
+        <c:axId val="55825780"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1875,7 +1875,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75141790"/>
+        <c:crossAx val="82286716"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1902,7 +1902,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2030,11 +2030,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="60942422"/>
-        <c:axId val="77316897"/>
+        <c:axId val="7427777"/>
+        <c:axId val="17323115"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="60942422"/>
+        <c:axId val="7427777"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2099,7 +2099,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77316897"/>
+        <c:crossAx val="17323115"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2107,7 +2107,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77316897"/>
+        <c:axId val="17323115"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2181,7 +2181,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60942422"/>
+        <c:crossAx val="7427777"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2208,7 +2208,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2336,11 +2336,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="71972965"/>
-        <c:axId val="65715879"/>
+        <c:axId val="9016580"/>
+        <c:axId val="71205806"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="71972965"/>
+        <c:axId val="9016580"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2405,7 +2405,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65715879"/>
+        <c:crossAx val="71205806"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2413,7 +2413,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65715879"/>
+        <c:axId val="71205806"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2487,7 +2487,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71972965"/>
+        <c:crossAx val="9016580"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2514,7 +2514,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2642,11 +2642,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="54942372"/>
-        <c:axId val="98092174"/>
+        <c:axId val="27325897"/>
+        <c:axId val="80895127"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="54942372"/>
+        <c:axId val="27325897"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2711,7 +2711,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98092174"/>
+        <c:crossAx val="80895127"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2719,7 +2719,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98092174"/>
+        <c:axId val="80895127"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2793,7 +2793,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54942372"/>
+        <c:crossAx val="27325897"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2820,7 +2820,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2948,11 +2948,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="73341775"/>
-        <c:axId val="53002710"/>
+        <c:axId val="93839920"/>
+        <c:axId val="90687836"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="73341775"/>
+        <c:axId val="93839920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3017,7 +3017,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53002710"/>
+        <c:crossAx val="90687836"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3025,7 +3025,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53002710"/>
+        <c:axId val="90687836"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3099,7 +3099,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73341775"/>
+        <c:crossAx val="93839920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3126,7 +3126,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3254,11 +3254,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="14283903"/>
-        <c:axId val="63599727"/>
+        <c:axId val="80166369"/>
+        <c:axId val="11912586"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="14283903"/>
+        <c:axId val="80166369"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3323,7 +3323,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63599727"/>
+        <c:crossAx val="11912586"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3331,7 +3331,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63599727"/>
+        <c:axId val="11912586"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3405,7 +3405,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14283903"/>
+        <c:crossAx val="80166369"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9297,7 +9297,7 @@
   <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B10" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>